<commit_message>
update grid search table
</commit_message>
<xml_diff>
--- a/Output/Classifier Fitting/Grid Search Table.xlsx
+++ b/Output/Classifier Fitting/Grid Search Table.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,170 +558,272 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>SVM</t>
+          <t>Random Forest</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>c_values</t>
+          <t>n_estimators</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>0.09999999999999999, 1.0, 10.0, 100.0</t>
+          <t>500, 1000, 1500</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>SVM</t>
+          <t>Random Forest</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>kernel_grid</t>
+          <t>max_features</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>rbf, poly</t>
+          <t>sqrt</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>SVM</t>
+          <t>Random Forest</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>gamma_grid</t>
+          <t>max_depth</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>0.09999999999999999, 1.0, 10.0, 100.0</t>
+          <t>20, 40, 60, 80</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>SVM</t>
+          <t>Random Forest</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>degree_grid</t>
+          <t>bootstrap</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>2, 3, 5, 7</t>
+          <t>True, False</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>SVM</t>
+          <t>Random Forest</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>k_folds</t>
+          <t>min_samples_leaf</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1, 2</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>XGBoost</t>
+          <t>SVM</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>learning_rate</t>
+          <t>c_values</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>0.01, 0.1, 0.3</t>
+          <t>0.01, 0.1, 1, 10</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>XGBoost</t>
+          <t>SVM</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>n_estimators</t>
+          <t>kernel_grid</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>100, 200</t>
+          <t>rbf, poly</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>XGBoost</t>
+          <t>SVM</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>max_depth</t>
+          <t>gamma_grid</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>3, 6</t>
+          <t>0.001, 0.01, 0.1, 1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>XGBoost</t>
+          <t>SVM</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>subsample</t>
+          <t>degree_grid</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>0.8, 1</t>
+          <t>2, 4</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>class_weight</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>balanced, None</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>k_folds</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
           <t>XGBoost</t>
         </is>
       </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>colsample_bytree</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>0.8, 1</t>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>n_estimators</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>100, 200, 300</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>learning_rate</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>0.1, 0.3, 0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>max_depth</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>2, 3, 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>min_child_weight</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>1, 3, 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>k_folds</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
clean up decimal places in tables
</commit_message>
<xml_diff>
--- a/Output/Classifier Fitting/Grid Search Table.xlsx
+++ b/Output/Classifier Fitting/Grid Search Table.xlsx
@@ -653,7 +653,7 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>0.01, 0.31622776601683794, 10.0</t>
+          <t>0.01, 0.32, 10.0</t>
         </is>
       </c>
     </row>
@@ -687,7 +687,7 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>1e-05, 0.00025118864315095795, 0.00630957344480193, 0.1584893192461111, 3.981071705534969, 100.0, scale</t>
+          <t>1e-05, 2.51e-04, 6.31e-03, 0.16, 3.98, 100.0, scale</t>
         </is>
       </c>
     </row>

</xml_diff>